<commit_message>
11.24 batch-temp.md this was a modification and implementation of this process that differed from the other branch. Namely, in that config and blacklist names were not asked to be altered.
</commit_message>
<xml_diff>
--- a/Batchdata/template_config.xlsx
+++ b/Batchdata/template_config.xlsx
@@ -661,7 +661,6 @@
           <t>defaults.state_fallback</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>2-letter</t>
@@ -805,102 +804,102 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>record_id</t>
+          <t>BD_RECORD_ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>source_type</t>
+          <t>BD_SOURCE_TYPE</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>source_entity_name</t>
+          <t>BD_ENTITY_NAME</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>source_entity_id</t>
+          <t>BD_SOURCE_ENTITY_ID</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>title_role</t>
+          <t>BD_TITLE_ROLE</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>target_first_name</t>
+          <t>BD_TARGET_FIRST_NAME</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>target_last_name</t>
+          <t>BD_TARGET_LAST_NAME</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>owner_name_full</t>
+          <t>BD_OWNER_NAME_FULL</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>address_line1</t>
+          <t>BD_ADDRESS</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>address_line2</t>
+          <t>BD_ADDRESS_2</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>BD_CITY</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>BD_STATE</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>zip</t>
+          <t>BD_ZIP</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>county</t>
+          <t>BD_COUNTY</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>apn</t>
+          <t>BD_APN</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>mailing_line1</t>
+          <t>BD_MAILING_LINE1</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>mailing_city</t>
+          <t>BD_MAILING_CITY</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>mailing_state</t>
+          <t>BD_MAILING_STATE</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>mailing_zip</t>
+          <t>BD_MAILING_ZIP</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>notes</t>
+          <t>BD_NOTES</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove some unneeded columns. Also a cleaner batchdata from ECorp. Next up, need to add some eCorp subordinates into batchdata and the rest of the needed in-batchdata, so no lost data or records.
</commit_message>
<xml_diff>
--- a/Batchdata/template_config.xlsx
+++ b/Batchdata/template_config.xlsx
@@ -661,6 +661,7 @@
           <t>defaults.state_fallback</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>2-letter</t>
@@ -793,7 +794,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,100 +805,185 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>FULL_ADDRESS</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>COUNTY</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Owner_Ownership</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_INDEX_#</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>OWNER_TYPE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_SEARCH_NAME</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_TYPE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_NAME_S</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_ENTITY_ID_S</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_ENTITY_TYPE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_STATUS</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_FORMATION_DATE</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_BUSINESS_TYPE</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_STATE</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_COUNTY</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_COMMENTS</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ECORP_URL</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>BD_RECORD_ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>BD_SOURCE_TYPE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>BD_ENTITY_NAME</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>BD_SOURCE_ENTITY_ID</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>BD_TITLE_ROLE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>BD_TARGET_FIRST_NAME</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>BD_TARGET_LAST_NAME</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>BD_OWNER_NAME_FULL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>BD_ADDRESS</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>BD_ADDRESS_2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>BD_CITY</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>BD_STATE</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>BD_ZIP</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>BD_COUNTY</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>BD_APN</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>BD_MAILING_LINE1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>BD_MAILING_CITY</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>BD_MAILING_STATE</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>BD_MAILING_ZIP</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>BD_NOTES</t>
         </is>

</xml_diff>